<commit_message>
feat: 1.0.31 seguridad y 2 cotizaciones
</commit_message>
<xml_diff>
--- a/backend/docs/EVA-EST.xlsx
+++ b/backend/docs/EVA-EST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\planosperu-app\backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694D8912-811F-4C3D-B35F-B39E2CBBFD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD181C0-0F63-4236-B6A4-F1A61DAC87B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7AF56AFE-BDCB-4CF7-AA6B-4FA438D0E0D4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="EVA-EST" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'EVA-EST'!$A$1:$H$74</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'EVA-EST'!$A$1:$H$72</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t xml:space="preserve">                                                                                                                  </t>
   </si>
@@ -68,15 +68,9 @@
     <t>https://www.planosperu.com.pe</t>
   </si>
   <si>
-    <t>COTIZACIÓN / CONTRATO DE EVALUACIÓN ESTRUCTURAL</t>
-  </si>
-  <si>
     <t>Proyecto:</t>
   </si>
   <si>
-    <t>Levantamiento Estructural de los Edificios</t>
-  </si>
-  <si>
     <t>Detalles:</t>
   </si>
   <si>
@@ -113,13 +107,7 @@
     <t>B.6 ESTUDIO DESTRUCTIVO DE LOS PUNTOS</t>
   </si>
   <si>
-    <t>A.1 Inspección Ocular</t>
-  </si>
-  <si>
     <t>Red de tomacorrientes/Tableros/Medidores/Cuadro de</t>
-  </si>
-  <si>
-    <t>A.2 Verificación del Inmueble</t>
   </si>
   <si>
     <t>Cargas/Diagrama Unifilares/Pozo de Tierra, detalles</t>
@@ -181,46 +169,6 @@
         <rFont val="Arial Narrow"/>
         <family val="2"/>
       </rPr>
-      <t>B.2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="2" tint="-0.249977111117893"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="2" tint="-0.249977111117893"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ARQUITECTURA: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="2" tint="-0.249977111117893"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Distribucion de Ambientes/Medidas </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="2" tint="-0.249977111117893"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
       <t xml:space="preserve">B.8 INSTALACIONES DE GAS NATURAL: </t>
     </r>
     <r>
@@ -238,46 +186,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tuberias, Alimentacion, Cocina y Terma a Gas, detalles </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="2" tint="-0.249977111117893"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>B.3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="2" tint="-0.249977111117893"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="2" tint="-0.249977111117893"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CORTES Y ELEVACIONES: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="2" tint="-0.249977111117893"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Alturas de Ambientes,</t>
-    </r>
   </si>
   <si>
     <r>
@@ -320,20 +228,257 @@
     </r>
   </si>
   <si>
-    <t>Escaleras, Vigas y Niveles</t>
-  </si>
-  <si>
     <t xml:space="preserve">Instalacion de Timbre, Intercomunicador /Red TV /Fibra optica/cable
 </t>
   </si>
   <si>
-    <t>B.4 PLANOS ESTRUCTURALES</t>
-  </si>
-  <si>
     <t>B.10 UBICACIÓN Y LOCALIZACION</t>
   </si>
   <si>
-    <t>/Zapatas/Columnas/Cisterna y Detalle de Construcción</t>
+    <t>DISEÑO DE CORTESIA</t>
+  </si>
+  <si>
+    <t>C.  Elaboración de Documentos: del Expediente Solicitado</t>
+  </si>
+  <si>
+    <t>C.1 Lectura Titulo SUNARP</t>
+  </si>
+  <si>
+    <t>C.13 Presupuesto de Obra</t>
+  </si>
+  <si>
+    <t>C.2 Solicitud y Memoria Descriptiva SUNARP</t>
+  </si>
+  <si>
+    <t>C.14 Carta de Seguridad de Obra</t>
+  </si>
+  <si>
+    <t>C.3 Elaboracion de reglamento interno y junta de propietarios</t>
+  </si>
+  <si>
+    <t>C.15 Carta de Responsabilidad de Obra</t>
+  </si>
+  <si>
+    <t>C.4 Formulario Registral Nº 2</t>
+  </si>
+  <si>
+    <t>C.16 Informe técnico de conclusiones y recomendaciones</t>
+  </si>
+  <si>
+    <t>B.6 Modificación - Reglamento interno y junta de Propietarios</t>
+  </si>
+  <si>
+    <t>C.17 Independización de autoavaluo en 6 unidades en municipio</t>
+  </si>
+  <si>
+    <t>C.18 Escritura publica de abjudicacion predio a c/propietario</t>
+  </si>
+  <si>
+    <t>C.8 Declaracion Jurada</t>
+  </si>
+  <si>
+    <t>C.19 Asesoria durante el proceso</t>
+  </si>
+  <si>
+    <t>C.9 Anexo Nº 1 SUNARP</t>
+  </si>
+  <si>
+    <t>C.20 Memoria de Calculo de ETABS</t>
+  </si>
+  <si>
+    <t>C.10 Anexo Nº 4 SUNARP</t>
+  </si>
+  <si>
+    <t>C.21 Factibilidad Sanitaria</t>
+  </si>
+  <si>
+    <t>C.11 Subsanacion de observaciones Municipio (si hubiere)</t>
+  </si>
+  <si>
+    <t>C.22 Memoria descriptiva</t>
+  </si>
+  <si>
+    <t>C.12 FUE (Formulario Unico de Edifcaciones)</t>
+  </si>
+  <si>
+    <t>C.23 Factibilidad Electrica</t>
+  </si>
+  <si>
+    <t>2.- ALCANCES: ENTREGA DE DOCUMENTOS FIRMADOS – PROFESIONALES VIGENTES</t>
+  </si>
+  <si>
+    <t>2.3 Investigacion Antecedentes de Inmueble SUNARP</t>
+  </si>
+  <si>
+    <t>2.4 Servicio de Tramitación de expediente ante</t>
+  </si>
+  <si>
+    <t>la entidad correspondiente hasta la emision de la</t>
+  </si>
+  <si>
+    <t>licencia municipal</t>
+  </si>
+  <si>
+    <t>Observaciones:</t>
+  </si>
+  <si>
+    <t>3.-TIEMPO DE ELABORACION:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o Planos y/o Documentos </t>
+  </si>
+  <si>
+    <t>días hábiles.</t>
+  </si>
+  <si>
+    <t>4.-OFERTA TÉCNICA:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Costo del Proyecto   S/</t>
+  </si>
+  <si>
+    <t>Soles.</t>
+  </si>
+  <si>
+    <t>5.-MODO DE CANCELACIÓN:</t>
+  </si>
+  <si>
+    <t>Aprox.</t>
+  </si>
+  <si>
+    <t>NOTAS: Oferta Valida 7 Días, No incluye costo de impuesto alguno en la realización del trámite. Documento con vigencia limitada</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>STAFF DE PROFESIONALES:</t>
+  </si>
+  <si>
+    <t>Abog.Ljubica Nada Sékula Delgado CAD 18346</t>
+  </si>
+  <si>
+    <t>Ing. Civil Juan Manuel Leveau Guerra Nº CIP: 74155</t>
+  </si>
+  <si>
+    <t>Abog. Rommy Alberto Granda Montes CAL.S N° 01508</t>
+  </si>
+  <si>
+    <t>Ing. Eléctrico Daniel Adolfo Quispe Yupa CIP: 59744</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arq. Rodolfo Wilber Mogrovejo Huamani CAP N° 24431 </t>
+  </si>
+  <si>
+    <t>Ing. Sanitario José Francisco Javier Zela Steban CIP: 130333</t>
+  </si>
+  <si>
+    <t>A la Aprobación de la Presente Proforma y Medición del Inmueble</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuota 1 S/  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuota 2 S/  </t>
+  </si>
+  <si>
+    <t>Ing. Aguirre Alanya Luis Antonio CIP: 323997 CIV: 022178VCZRIX</t>
+  </si>
+  <si>
+    <t>Pisos:</t>
+  </si>
+  <si>
+    <t>Previo a la Contraentrega del Informe Técnico evaluac.</t>
+  </si>
+  <si>
+    <t>2.1 Planos Completos Firmados y Sellados 2 originales por Profesional Colegiado y Habilitado Vigente</t>
+  </si>
+  <si>
+    <t>B.10 SIMULACIÓN DE RESISTENCIA ESTRUCTURAL 3D</t>
+  </si>
+  <si>
+    <t>A.1 Planos - bosquejo del cliente</t>
+  </si>
+  <si>
+    <t>A.2 Medición de terreno o inmueble del cliente</t>
+  </si>
+  <si>
+    <t>Evaluación Estructural</t>
+  </si>
+  <si>
+    <t>COTIZACIÓN / CONTRATO DE EVALUACIÓN ESTRUCTURAL DE UN INMUEBLE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>B.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ARQUITECTURA: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Distribucion de Ambientes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>B.3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CORTES Y ELEVACIONES: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Alturas de Ambientes, Escaleras, Vigas y Niveles</t>
+    </r>
   </si>
   <si>
     <r>
@@ -360,194 +505,32 @@
         <rFont val="Arial Narrow"/>
         <family val="2"/>
       </rPr>
-      <t>ESTUDIO DESTRUCTIVO DE 45 PUNTOS</t>
+      <t xml:space="preserve">ESTRUCTURAS TECHOS ALIGERADOS: </t>
     </r>
-  </si>
-  <si>
-    <t>DISEÑO DE CORTESIA</t>
-  </si>
-  <si>
-    <t>Principales/Secundarias/Union de Vigas/Losas/Aceros</t>
-  </si>
-  <si>
-    <t>B.10 MODELADO ESCTRUCTURAL SISMICA (ETABS, SAP2000, LIBRE)</t>
-  </si>
-  <si>
-    <t>B.6 ESTUDIO CON DIAMANTINA DE 45 PUNTOS</t>
-  </si>
-  <si>
-    <t>C.  Elaboración de Documentos: del Expediente Solicitado</t>
-  </si>
-  <si>
-    <t>C.1 Lectura Titulo SUNARP</t>
-  </si>
-  <si>
-    <t>C.13 Presupuesto de Obra</t>
-  </si>
-  <si>
-    <t>C.2 Solicitud y Memoria Descriptiva SUNARP</t>
-  </si>
-  <si>
-    <t>C.14 Carta de Seguridad de Obra</t>
-  </si>
-  <si>
-    <t>C.3 Elaboracion de reglamento interno y junta de propietarios</t>
-  </si>
-  <si>
-    <t>C.15 Carta de Responsabilidad de Obra</t>
-  </si>
-  <si>
-    <t>C.4 Formulario Registral Nº 2</t>
-  </si>
-  <si>
-    <t>C.16 Informe técnico de conclusiones y recomendaciones</t>
-  </si>
-  <si>
-    <t>B.6 Modificación - Reglamento interno y junta de Propietarios</t>
-  </si>
-  <si>
-    <t>C.17 Independización de autoavaluo en 6 unidades en municipio</t>
-  </si>
-  <si>
-    <t>C.7 Informe Tecnico de Verificación</t>
-  </si>
-  <si>
-    <t>C.18 Escritura publica de abjudicacion predio a c/propietario</t>
-  </si>
-  <si>
-    <t>C.8 Declaracion Jurada</t>
-  </si>
-  <si>
-    <t>C.19 Asesoria durante el proceso</t>
-  </si>
-  <si>
-    <t>C.9 Anexo Nº 1 SUNARP</t>
-  </si>
-  <si>
-    <t>C.20 Memoria de Calculo de ETABS</t>
-  </si>
-  <si>
-    <t>C.10 Anexo Nº 4 SUNARP</t>
-  </si>
-  <si>
-    <t>C.21 Factibilidad Sanitaria</t>
-  </si>
-  <si>
-    <t>C.11 Subsanacion de observaciones Municipio (si hubiere)</t>
-  </si>
-  <si>
-    <t>C.22 Memoria descriptiva</t>
-  </si>
-  <si>
-    <t>C.12 FUE (Formulario Unico de Edifcaciones)</t>
-  </si>
-  <si>
-    <t>C.23 Factibilidad Electrica</t>
-  </si>
-  <si>
-    <t>2.- ALCANCES: ENTREGA DE DOCUMENTOS FIRMADOS – PROFESIONALES VIGENTES</t>
-  </si>
-  <si>
-    <t>2.1 Planos y Documentos Firmados y Sellados por Profesional Colegiado y Habilitado Vigente</t>
-  </si>
-  <si>
-    <t>2.3 Investigacion Antecedentes de Inmueble SUNARP</t>
-  </si>
-  <si>
-    <t>2.4 Servicio de Tramitación de expediente ante</t>
-  </si>
-  <si>
-    <t>la entidad correspondiente hasta la emision de la</t>
-  </si>
-  <si>
-    <t>2.2 CD - Grabación Digital del Planos</t>
-  </si>
-  <si>
-    <t>licencia municipal</t>
-  </si>
-  <si>
-    <t>Observaciones:</t>
-  </si>
-  <si>
-    <t>3.-TIEMPO DE ELABORACION:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">o Planos y/o Documentos </t>
-  </si>
-  <si>
-    <t>días hábiles.</t>
-  </si>
-  <si>
-    <t>4.-OFERTA TÉCNICA:</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Costo del Proyecto   S/</t>
-  </si>
-  <si>
-    <t>Soles.</t>
-  </si>
-  <si>
-    <t>5.-MODO DE CANCELACIÓN:</t>
-  </si>
-  <si>
-    <t>Al diagnostico de los Puntos a Evaluar</t>
-  </si>
-  <si>
-    <t>Aprox.</t>
-  </si>
-  <si>
-    <t>Al termino de Evaluación de los 90 Puntos</t>
-  </si>
-  <si>
-    <t>A la contra-entrega de Planos y Documentos Finalizados</t>
-  </si>
-  <si>
-    <t>NOTAS: Oferta Valida 7 Días, No incluye costo de impuesto alguno en la realización del trámite. Documento con vigencia limitada</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>STAFF DE PROFESIONALES:</t>
-  </si>
-  <si>
-    <t>Abog.Ljubica Nada Sékula Delgado CAD 18346</t>
-  </si>
-  <si>
-    <t>Ing. Civil Juan Manuel Leveau Guerra Nº CIP: 74155</t>
-  </si>
-  <si>
-    <t>Abog. Rommy Alberto Granda Montes CAL.S N° 01508</t>
-  </si>
-  <si>
-    <t>Ing. Eléctrico Daniel Adolfo Quispe Yupa CIP: 59744</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arq. Rodolfo Wilber Mogrovejo Huamani CAP N° 24431 </t>
-  </si>
-  <si>
-    <t>Ing. Sanitario José Francisco Javier Zela Steban CIP: 130333</t>
-  </si>
-  <si>
-    <t>A la Aprobación de la Presente Proforma y Medición del Inmueble</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cuota 1 S/  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cuota 2 S/  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cuota 3 S/  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cuota 4 S/  </t>
-  </si>
-  <si>
-    <t>Ing. Aguirre Alanya Luis Antonio CIP: 323997 CIV: 022178VCZRIX</t>
-  </si>
-  <si>
-    <t>Pisos:</t>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Vigas Principales/Secundarias/Union de vigas/Losas/Aceros Estribos, detalles</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B.4 ESTRUCTURAS DE CIMENTACIÓN: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Cimiento corrido /Zapatas/Columnas y Detalle de Construcción</t>
+    </r>
+  </si>
+  <si>
+    <t>C.7 Informe Técnico de Evaluación y Diagnostico Final</t>
   </si>
 </sst>
 </file>
@@ -872,7 +855,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -998,14 +981,262 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1038,302 +1269,69 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1715,13 +1713,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>204493</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>67408</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2006,7 +2004,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>285941</xdr:colOff>
+      <xdr:colOff>285942</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>63792</xdr:rowOff>
     </xdr:to>
@@ -2351,16 +2349,16 @@
     <tabColor theme="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A3:H76"/>
+  <dimension ref="A3:H74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A62" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67:E67"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58:G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" customWidth="1"/>
@@ -2376,168 +2374,168 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="135" t="s">
+      <c r="D4" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="135"/>
-      <c r="F4" s="135"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="136" t="s">
+      <c r="D5" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="137" t="s">
+      <c r="D6" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="137"/>
-      <c r="F6" s="137"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="138" t="s">
+      <c r="D7" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="138"/>
-      <c r="F7" s="138"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="139"/>
-      <c r="B8" s="139"/>
-      <c r="C8" s="139"/>
-      <c r="D8" s="139"/>
-      <c r="E8" s="139"/>
-      <c r="F8" s="139"/>
-      <c r="G8" s="139"/>
-      <c r="H8" s="139"/>
+      <c r="A8" s="45"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
     </row>
     <row r="9" spans="1:8" s="5" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="134" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="134"/>
-      <c r="D9" s="134"/>
-      <c r="E9" s="134"/>
-      <c r="F9" s="134"/>
-      <c r="G9" s="134"/>
+      <c r="B9" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="134"/>
-      <c r="C10" s="134"/>
-      <c r="D10" s="134"/>
-      <c r="E10" s="134"/>
-      <c r="F10" s="134"/>
-      <c r="G10" s="134"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="B11" s="123" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="123"/>
-      <c r="D11" s="123"/>
-      <c r="E11" s="123"/>
-      <c r="F11" s="8" t="s">
-        <v>12</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="123"/>
-      <c r="C12" s="123"/>
-      <c r="D12" s="123"/>
-      <c r="E12" s="123"/>
-      <c r="F12" s="123"/>
-      <c r="G12" s="123"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
-      <c r="B13" s="123"/>
-      <c r="C13" s="123"/>
-      <c r="D13" s="123"/>
-      <c r="E13" s="123"/>
-      <c r="F13" s="123"/>
-      <c r="G13" s="123"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="B14" s="39"/>
       <c r="C14" s="13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="123"/>
-      <c r="C15" s="123"/>
-      <c r="D15" s="123"/>
-      <c r="E15" s="123"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
       <c r="F15" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
-      <c r="B16" s="124"/>
-      <c r="C16" s="124"/>
-      <c r="D16" s="124"/>
-      <c r="E16" s="124"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
       <c r="F16" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="123"/>
-      <c r="C17" s="123"/>
+        <v>17</v>
+      </c>
+      <c r="B17" s="51"/>
+      <c r="C17" s="51"/>
       <c r="D17" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E17" s="19">
         <f ca="1">TODAY()</f>
-        <v>45849</v>
+        <v>45853</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
@@ -2545,502 +2543,492 @@
     </row>
     <row r="18" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
-      <c r="B18" s="125"/>
-      <c r="C18" s="125"/>
-      <c r="D18" s="125"/>
-      <c r="E18" s="125"/>
-      <c r="F18" s="125"/>
-      <c r="G18" s="125"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
       <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
-      <c r="B19" s="126" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="127"/>
-      <c r="D19" s="128"/>
-      <c r="E19" s="129"/>
-      <c r="F19" s="130"/>
+      <c r="B19" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="55"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="58"/>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
     </row>
     <row r="20" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
-      <c r="B20" s="126" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="127"/>
-      <c r="D20" s="127"/>
-      <c r="E20" s="131" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="132"/>
-      <c r="G20" s="133"/>
+      <c r="B20" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="130" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="131"/>
+      <c r="G20" s="132"/>
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
-      <c r="B21" s="121" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="122"/>
-      <c r="D21" s="122"/>
-      <c r="E21" s="97" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="98"/>
-      <c r="G21" s="99"/>
+      <c r="B21" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="49"/>
+      <c r="G21" s="50"/>
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
-      <c r="B22" s="116" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="117"/>
-      <c r="D22" s="117"/>
-      <c r="E22" s="97" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="98"/>
-      <c r="G22" s="99"/>
+      <c r="B22" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="49"/>
+      <c r="G22" s="50"/>
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
-      <c r="B23" s="66" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="97" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" s="98"/>
-      <c r="G23" s="99"/>
+      <c r="B23" s="61" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="49"/>
+      <c r="G23" s="50"/>
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
-      <c r="B24" s="118" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="119"/>
-      <c r="D24" s="120"/>
-      <c r="E24" s="97" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" s="98"/>
-      <c r="G24" s="99"/>
+      <c r="B24" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="64"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="49"/>
+      <c r="G24" s="50"/>
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
-      <c r="B25" s="97" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="98"/>
-      <c r="D25" s="99"/>
-      <c r="E25" s="97" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="98"/>
-      <c r="G25" s="99"/>
+      <c r="B25" s="74" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="71"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="49"/>
+      <c r="G25" s="50"/>
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
-      <c r="B26" s="97" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="98"/>
-      <c r="D26" s="99"/>
-      <c r="E26" s="97" t="s">
-        <v>35</v>
-      </c>
-      <c r="F26" s="98"/>
-      <c r="G26" s="99"/>
+      <c r="B26" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="49"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="49"/>
+      <c r="G26" s="50"/>
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
-      <c r="B27" s="97" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="98"/>
-      <c r="D27" s="99"/>
-      <c r="E27" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="98"/>
-      <c r="G27" s="99"/>
+      <c r="B27" s="107" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="136"/>
+      <c r="D27" s="109"/>
+      <c r="E27" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="49"/>
+      <c r="G27" s="50"/>
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
-      <c r="B28" s="97" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="98"/>
-      <c r="D28" s="99"/>
-      <c r="E28" s="57" t="s">
-        <v>39</v>
-      </c>
-      <c r="F28" s="58"/>
-      <c r="G28" s="59"/>
+      <c r="B28" s="107"/>
+      <c r="C28" s="136"/>
+      <c r="D28" s="109"/>
+      <c r="E28" s="68" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="69"/>
+      <c r="G28" s="70"/>
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
-      <c r="B29" s="100" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="101"/>
-      <c r="D29" s="102"/>
-      <c r="E29" s="103" t="s">
-        <v>41</v>
-      </c>
-      <c r="F29" s="98"/>
-      <c r="G29" s="99"/>
+      <c r="B29" s="75" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="137"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="73" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="49"/>
+      <c r="G29" s="50"/>
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
-      <c r="B30" s="97" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="98"/>
-      <c r="D30" s="99"/>
-      <c r="E30" s="97"/>
-      <c r="F30" s="98"/>
-      <c r="G30" s="99"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="137"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="50"/>
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27"/>
-      <c r="B31" s="104" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="101"/>
-      <c r="D31" s="102"/>
-      <c r="E31" s="105" t="s">
-        <v>44</v>
-      </c>
-      <c r="F31" s="106"/>
-      <c r="G31" s="107"/>
+      <c r="B31" s="107" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="136"/>
+      <c r="D31" s="109"/>
+      <c r="E31" s="141" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="142"/>
+      <c r="G31" s="143"/>
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
-      <c r="B32" s="97" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="98"/>
-      <c r="D32" s="99"/>
-      <c r="E32" s="108" t="s">
-        <v>46</v>
-      </c>
-      <c r="F32" s="109"/>
-      <c r="G32" s="110"/>
+      <c r="B32" s="107"/>
+      <c r="C32" s="136"/>
+      <c r="D32" s="109"/>
+      <c r="E32" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="F32" s="76"/>
+      <c r="G32" s="77"/>
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
-      <c r="B33" s="114" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" s="115"/>
-      <c r="D33" s="115"/>
-      <c r="E33" s="111"/>
-      <c r="F33" s="112"/>
-      <c r="G33" s="113"/>
+      <c r="B33" s="138"/>
+      <c r="C33" s="139"/>
+      <c r="D33" s="140"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="79"/>
+      <c r="G33" s="80"/>
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
-      <c r="B34" s="66" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="67"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="95"/>
-      <c r="F34" s="95"/>
-      <c r="G34" s="96"/>
+      <c r="B34" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="67"/>
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
-      <c r="B35" s="89" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35" s="90"/>
-      <c r="D35" s="91"/>
-      <c r="E35" s="75" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="76"/>
-      <c r="G35" s="77"/>
+      <c r="B35" s="81" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="82"/>
+      <c r="D35" s="83"/>
+      <c r="E35" s="84" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" s="85"/>
+      <c r="G35" s="86"/>
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
-      <c r="B36" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="55"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="92" t="s">
-        <v>52</v>
-      </c>
-      <c r="F36" s="93"/>
-      <c r="G36" s="94"/>
+      <c r="B36" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="88"/>
+      <c r="D36" s="89"/>
+      <c r="E36" s="90" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="91"/>
+      <c r="G36" s="92"/>
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
-      <c r="B37" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="C37" s="55"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="92" t="s">
-        <v>54</v>
-      </c>
-      <c r="F37" s="93"/>
-      <c r="G37" s="94"/>
+      <c r="B37" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="88"/>
+      <c r="D37" s="89"/>
+      <c r="E37" s="127" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" s="128"/>
+      <c r="G37" s="129"/>
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
-      <c r="B38" s="54" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38" s="55"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="83" t="s">
-        <v>56</v>
-      </c>
-      <c r="F38" s="84"/>
-      <c r="G38" s="85"/>
+      <c r="B38" s="87" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="88"/>
+      <c r="D38" s="89"/>
+      <c r="E38" s="127" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="128"/>
+      <c r="G38" s="129"/>
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
-      <c r="B39" s="54" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39" s="55"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="54" t="s">
-        <v>58</v>
-      </c>
-      <c r="F39" s="55"/>
-      <c r="G39" s="56"/>
+      <c r="B39" s="87" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="88"/>
+      <c r="D39" s="89"/>
+      <c r="E39" s="127" t="s">
+        <v>45</v>
+      </c>
+      <c r="F39" s="128"/>
+      <c r="G39" s="129"/>
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
-      <c r="B40" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="C40" s="55"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="F40" s="55"/>
-      <c r="G40" s="56"/>
+      <c r="B40" s="93" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="94"/>
+      <c r="D40" s="95"/>
+      <c r="E40" s="127" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" s="128"/>
+      <c r="G40" s="129"/>
       <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="54" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" s="55"/>
-      <c r="D41" s="56"/>
-      <c r="E41" s="83" t="s">
-        <v>62</v>
-      </c>
-      <c r="F41" s="84"/>
-      <c r="G41" s="85"/>
+      <c r="B41" s="87" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="88"/>
+      <c r="D41" s="89"/>
+      <c r="E41" s="127" t="s">
+        <v>48</v>
+      </c>
+      <c r="F41" s="128"/>
+      <c r="G41" s="129"/>
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
-      <c r="B42" s="54" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="55"/>
-      <c r="D42" s="56"/>
-      <c r="E42" s="86" t="s">
-        <v>64</v>
-      </c>
-      <c r="F42" s="87"/>
-      <c r="G42" s="88"/>
+      <c r="B42" s="87" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="88"/>
+      <c r="D42" s="89"/>
+      <c r="E42" s="133" t="s">
+        <v>50</v>
+      </c>
+      <c r="F42" s="134"/>
+      <c r="G42" s="135"/>
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
-      <c r="B43" s="54" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="55"/>
-      <c r="D43" s="56"/>
-      <c r="E43" s="57" t="s">
-        <v>66</v>
-      </c>
-      <c r="F43" s="58"/>
-      <c r="G43" s="59"/>
+      <c r="B43" s="87" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" s="88"/>
+      <c r="D43" s="89"/>
+      <c r="E43" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="F43" s="69"/>
+      <c r="G43" s="70"/>
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
-      <c r="B44" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="C44" s="55"/>
-      <c r="D44" s="56"/>
-      <c r="E44" s="57" t="s">
-        <v>68</v>
-      </c>
-      <c r="F44" s="58"/>
-      <c r="G44" s="59"/>
+      <c r="B44" s="87" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="88"/>
+      <c r="D44" s="89"/>
+      <c r="E44" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="F44" s="69"/>
+      <c r="G44" s="70"/>
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
-      <c r="B45" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="C45" s="61"/>
-      <c r="D45" s="62"/>
-      <c r="E45" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="F45" s="64"/>
-      <c r="G45" s="65"/>
+      <c r="B45" s="97" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="98"/>
+      <c r="D45" s="99"/>
+      <c r="E45" s="100" t="s">
+        <v>56</v>
+      </c>
+      <c r="F45" s="101"/>
+      <c r="G45" s="102"/>
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="66" t="s">
-        <v>71</v>
-      </c>
-      <c r="C46" s="67"/>
-      <c r="D46" s="67"/>
-      <c r="E46" s="67"/>
-      <c r="F46" s="67"/>
-      <c r="G46" s="68"/>
+      <c r="B46" s="61" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="62"/>
+      <c r="D46" s="62"/>
+      <c r="E46" s="62"/>
+      <c r="F46" s="62"/>
+      <c r="G46" s="103"/>
     </row>
     <row r="47" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="69" t="s">
-        <v>72</v>
-      </c>
-      <c r="C47" s="70"/>
-      <c r="D47" s="71"/>
-      <c r="E47" s="75" t="s">
-        <v>73</v>
-      </c>
-      <c r="F47" s="76"/>
-      <c r="G47" s="77"/>
+      <c r="B47" s="104" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="105"/>
+      <c r="D47" s="106"/>
+      <c r="E47" s="84" t="s">
+        <v>58</v>
+      </c>
+      <c r="F47" s="85"/>
+      <c r="G47" s="86"/>
     </row>
     <row r="48" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="72"/>
-      <c r="C48" s="73"/>
-      <c r="D48" s="74"/>
-      <c r="E48" s="54" t="s">
-        <v>74</v>
-      </c>
-      <c r="F48" s="55"/>
-      <c r="G48" s="56"/>
+      <c r="B48" s="107"/>
+      <c r="C48" s="108"/>
+      <c r="D48" s="109"/>
+      <c r="E48" s="87" t="s">
+        <v>59</v>
+      </c>
+      <c r="F48" s="88"/>
+      <c r="G48" s="89"/>
     </row>
     <row r="49" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="72"/>
-      <c r="C49" s="73"/>
-      <c r="D49" s="74"/>
-      <c r="E49" s="54" t="s">
-        <v>75</v>
-      </c>
-      <c r="F49" s="55"/>
-      <c r="G49" s="56"/>
+      <c r="B49" s="107"/>
+      <c r="C49" s="108"/>
+      <c r="D49" s="109"/>
+      <c r="E49" s="87" t="s">
+        <v>60</v>
+      </c>
+      <c r="F49" s="88"/>
+      <c r="G49" s="89"/>
     </row>
     <row r="50" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="78" t="s">
-        <v>76</v>
-      </c>
-      <c r="C50" s="79"/>
-      <c r="D50" s="80"/>
-      <c r="E50" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="F50" s="61"/>
-      <c r="G50" s="62"/>
+      <c r="B50" s="110"/>
+      <c r="C50" s="111"/>
+      <c r="D50" s="112"/>
+      <c r="E50" s="97" t="s">
+        <v>61</v>
+      </c>
+      <c r="F50" s="98"/>
+      <c r="G50" s="99"/>
     </row>
     <row r="51" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="81"/>
-      <c r="C51" s="81"/>
-      <c r="D51" s="81"/>
-      <c r="E51" s="81"/>
-      <c r="F51" s="81"/>
-      <c r="G51" s="81"/>
+      <c r="B51" s="113"/>
+      <c r="C51" s="113"/>
+      <c r="D51" s="113"/>
+      <c r="E51" s="113"/>
+      <c r="F51" s="113"/>
+      <c r="G51" s="113"/>
     </row>
     <row r="52" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="C52" s="82"/>
-      <c r="D52" s="82"/>
-      <c r="E52" s="82"/>
-      <c r="F52" s="82"/>
-      <c r="G52" s="82"/>
+        <v>62</v>
+      </c>
+      <c r="C52" s="114"/>
+      <c r="D52" s="114"/>
+      <c r="E52" s="114"/>
+      <c r="F52" s="114"/>
+      <c r="G52" s="114"/>
     </row>
     <row r="53" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="53"/>
-      <c r="C53" s="53"/>
-      <c r="D53" s="53"/>
-      <c r="E53" s="53"/>
-      <c r="F53" s="53"/>
-      <c r="G53" s="53"/>
+      <c r="B53" s="96"/>
+      <c r="C53" s="96"/>
+      <c r="D53" s="96"/>
+      <c r="E53" s="96"/>
+      <c r="F53" s="96"/>
+      <c r="G53" s="96"/>
     </row>
     <row r="54" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="53"/>
-      <c r="C54" s="53"/>
-      <c r="D54" s="53"/>
-      <c r="E54" s="53"/>
-      <c r="F54" s="53"/>
-      <c r="G54" s="53"/>
+      <c r="B54" s="96"/>
+      <c r="C54" s="96"/>
+      <c r="D54" s="96"/>
+      <c r="E54" s="96"/>
+      <c r="F54" s="96"/>
+      <c r="G54" s="96"/>
     </row>
     <row r="55" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="44"/>
-      <c r="C55" s="44"/>
-      <c r="D55" s="44"/>
-      <c r="E55" s="44"/>
-      <c r="F55" s="44"/>
-      <c r="G55" s="44"/>
+      <c r="B55" s="116"/>
+      <c r="C55" s="116"/>
+      <c r="D55" s="116"/>
+      <c r="E55" s="116"/>
+      <c r="F55" s="116"/>
+      <c r="G55" s="116"/>
     </row>
     <row r="56" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="21"/>
-      <c r="B56" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="45"/>
-      <c r="G56" s="45"/>
+      <c r="B56" s="117" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" s="117"/>
+      <c r="D56" s="117"/>
+      <c r="E56" s="117"/>
+      <c r="F56" s="117"/>
+      <c r="G56" s="117"/>
       <c r="H56" s="22"/>
     </row>
     <row r="57" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="22"/>
-      <c r="B57" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="C57" s="46"/>
+      <c r="B57" s="118" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" s="118"/>
       <c r="D57" s="29">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E57" s="20" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="F57" s="20"/>
       <c r="G57" s="20"/>
@@ -3048,209 +3036,171 @@
     </row>
     <row r="58" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
-      <c r="B58" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="C58" s="45"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="45"/>
-      <c r="F58" s="45"/>
-      <c r="G58" s="45"/>
+      <c r="B58" s="117" t="s">
+        <v>66</v>
+      </c>
+      <c r="C58" s="117"/>
+      <c r="D58" s="117"/>
+      <c r="E58" s="117"/>
+      <c r="F58" s="117"/>
+      <c r="G58" s="117"/>
       <c r="H58" s="22"/>
     </row>
     <row r="59" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="22"/>
-      <c r="B59" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="C59" s="47"/>
+      <c r="B59" s="119" t="s">
+        <v>67</v>
+      </c>
+      <c r="C59" s="119"/>
       <c r="D59" s="31">
-        <f>C61+C62+C64</f>
+        <f>C61+C62</f>
         <v>0</v>
       </c>
-      <c r="E59" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="F59" s="48"/>
+      <c r="E59" s="120" t="s">
+        <v>68</v>
+      </c>
+      <c r="F59" s="120"/>
       <c r="G59" s="20"/>
       <c r="H59" s="22"/>
     </row>
     <row r="60" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="21"/>
-      <c r="B60" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="C60" s="45"/>
-      <c r="D60" s="45"/>
-      <c r="E60" s="45"/>
-      <c r="F60" s="45"/>
-      <c r="G60" s="45"/>
+      <c r="B60" s="117" t="s">
+        <v>69</v>
+      </c>
+      <c r="C60" s="117"/>
+      <c r="D60" s="117"/>
+      <c r="E60" s="117"/>
+      <c r="F60" s="117"/>
+      <c r="G60" s="117"/>
       <c r="H60" s="22"/>
     </row>
     <row r="61" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22"/>
       <c r="B61" s="30" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="C61" s="32"/>
-      <c r="D61" s="49" t="s">
-        <v>99</v>
-      </c>
-      <c r="E61" s="50"/>
-      <c r="F61" s="50"/>
+      <c r="D61" s="121" t="s">
+        <v>80</v>
+      </c>
+      <c r="E61" s="122"/>
+      <c r="F61" s="122"/>
       <c r="G61" s="33">
         <f ca="1">E$17</f>
-        <v>45849</v>
+        <v>45853</v>
       </c>
       <c r="H61" s="22"/>
     </row>
     <row r="62" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="22"/>
       <c r="B62" s="30" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C62" s="34"/>
-      <c r="D62" s="51" t="s">
-        <v>86</v>
-      </c>
-      <c r="E62" s="51"/>
-      <c r="F62" s="51"/>
+      <c r="D62" s="123" t="s">
+        <v>85</v>
+      </c>
+      <c r="E62" s="123"/>
+      <c r="F62" s="123"/>
       <c r="G62" s="33">
-        <f ca="1">E17+7</f>
-        <v>45856</v>
+        <f ca="1">E17+14</f>
+        <v>45867</v>
       </c>
       <c r="H62" s="35" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="22"/>
-      <c r="B63" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="C63" s="34"/>
-      <c r="D63" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="E63" s="52"/>
-      <c r="F63" s="52"/>
-      <c r="G63" s="33">
-        <f ca="1">E$17+35</f>
-        <v>45884</v>
-      </c>
-      <c r="H63" s="35" t="s">
-        <v>87</v>
-      </c>
+      <c r="A63" s="10"/>
+      <c r="B63" s="115" t="s">
+        <v>71</v>
+      </c>
+      <c r="C63" s="115"/>
+      <c r="D63" s="115"/>
+      <c r="E63" s="115"/>
+      <c r="F63" s="115"/>
+      <c r="G63" s="115"/>
+      <c r="H63" s="36"/>
     </row>
     <row r="64" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="22"/>
-      <c r="B64" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="C64" s="34"/>
-      <c r="D64" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="E64" s="51"/>
-      <c r="F64" s="51"/>
-      <c r="G64" s="33">
-        <f ca="1">E17+60</f>
-        <v>45909</v>
-      </c>
-      <c r="H64" s="35" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="10"/>
-      <c r="B65" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="C65" s="43"/>
-      <c r="D65" s="43"/>
-      <c r="E65" s="43"/>
-      <c r="F65" s="43"/>
-      <c r="G65" s="43"/>
-      <c r="H65" s="36"/>
-    </row>
-    <row r="66" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="B66" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="C66" s="41"/>
-      <c r="D66" s="41"/>
-      <c r="E66" s="41"/>
-      <c r="F66" s="41"/>
-      <c r="G66" s="41"/>
-      <c r="H66" s="23"/>
-    </row>
-    <row r="67" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C67" s="40"/>
-      <c r="D67" s="40"/>
-      <c r="E67" s="40"/>
-      <c r="F67" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="G67" s="40"/>
-      <c r="H67" s="40"/>
-    </row>
-    <row r="68" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="C68" s="42"/>
-      <c r="D68" s="42"/>
-      <c r="E68" s="42"/>
-      <c r="F68" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="G68" s="40"/>
-      <c r="H68" s="40"/>
-    </row>
-    <row r="69" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="42" t="s">
-        <v>96</v>
-      </c>
-      <c r="C69" s="42"/>
-      <c r="D69" s="42"/>
-      <c r="E69" s="42"/>
-      <c r="F69" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="G69" s="40"/>
-      <c r="H69" s="40"/>
-    </row>
-    <row r="70" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C70" s="40"/>
-      <c r="D70" s="40"/>
-      <c r="E70" s="40"/>
-      <c r="F70" s="40"/>
-      <c r="G70" s="40"/>
-      <c r="H70" s="40"/>
-    </row>
-    <row r="71" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="38"/>
-      <c r="C71" s="38"/>
-      <c r="D71" s="38"/>
-      <c r="E71" s="38"/>
-      <c r="F71" s="38"/>
-      <c r="G71" s="38"/>
-      <c r="H71" s="38"/>
-    </row>
-    <row r="72" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A64" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B64" s="125" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64" s="125"/>
+      <c r="D64" s="125"/>
+      <c r="E64" s="125"/>
+      <c r="F64" s="125"/>
+      <c r="G64" s="125"/>
+      <c r="H64" s="23"/>
+    </row>
+    <row r="65" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="124" t="s">
+        <v>83</v>
+      </c>
+      <c r="C65" s="124"/>
+      <c r="D65" s="124"/>
+      <c r="E65" s="124"/>
+      <c r="F65" s="124" t="s">
+        <v>74</v>
+      </c>
+      <c r="G65" s="124"/>
+      <c r="H65" s="124"/>
+    </row>
+    <row r="66" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="126" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" s="126"/>
+      <c r="D66" s="126"/>
+      <c r="E66" s="126"/>
+      <c r="F66" s="124" t="s">
+        <v>76</v>
+      </c>
+      <c r="G66" s="124"/>
+      <c r="H66" s="124"/>
+    </row>
+    <row r="67" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="126" t="s">
+        <v>77</v>
+      </c>
+      <c r="C67" s="126"/>
+      <c r="D67" s="126"/>
+      <c r="E67" s="126"/>
+      <c r="F67" s="124" t="s">
+        <v>78</v>
+      </c>
+      <c r="G67" s="124"/>
+      <c r="H67" s="124"/>
+    </row>
+    <row r="68" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="124" t="s">
+        <v>79</v>
+      </c>
+      <c r="C68" s="124"/>
+      <c r="D68" s="124"/>
+      <c r="E68" s="124"/>
+      <c r="F68" s="124"/>
+      <c r="G68" s="124"/>
+      <c r="H68" s="124"/>
+    </row>
+    <row r="69" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="38"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="38"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="38"/>
+      <c r="H69" s="38"/>
+    </row>
+    <row r="70" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="jRsd99E24Wg0cREusBHWfr8AogbmoKcBAiIEI/AkVrYZ6d3Zv1r365CvDnomnIuIagvCXHSwta3CL7/ZYpI/1A==" saltValue="4GoUJy3q9tod8g93O8nnng==" spinCount="100000" sqref="B17:C17 E17 G15 G16:H16 D14 B14 B13:H13" name="Rango1"/>
@@ -3264,68 +3214,26 @@
     <protectedRange algorithmName="SHA-512" hashValue="AvALmQbaBHPy/2D6NWeVBUXqKrVf5+JMiV0rv9ctsh3U+v+jJx3afL0wo26AWqHiVPRHYNv0n+KWylatMMGOjQ==" saltValue="Ch+TBLTSso8GOLDPE2CwFQ==" spinCount="100000" sqref="F33:G33" name="Rango1_8"/>
     <protectedRange algorithmName="SHA-512" hashValue="zUrWTGEZiJFMgzDqDTBlVt+5/9aQcTuJw4/Tg0qXKmOEBmnAPkc2PftdRKWEJAjo6Tejl/2GECle77oEWrFAIQ==" saltValue="IwcVdvVtxL7J72Vc6oLNHQ==" spinCount="100000" sqref="E51:G51" name="Rango1_6_1"/>
   </protectedRanges>
-  <mergeCells count="97">
-    <mergeCell ref="B9:G10"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:G33"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
+  <mergeCells count="91">
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="D62:F62"/>
     <mergeCell ref="B54:G54"/>
     <mergeCell ref="B44:D44"/>
     <mergeCell ref="E44:G44"/>
@@ -3341,34 +3249,70 @@
     <mergeCell ref="B51:G51"/>
     <mergeCell ref="C52:G52"/>
     <mergeCell ref="B53:G53"/>
-    <mergeCell ref="B65:G65"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="B66:G66"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="B69:E69"/>
-    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G33"/>
+    <mergeCell ref="B27:D28"/>
+    <mergeCell ref="B29:D30"/>
+    <mergeCell ref="B31:D33"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="B9:G10"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A8:H8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1" xr:uid="{235390CD-A36E-470F-A792-392322EAE957}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="91" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="90" orientation="portrait" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>